<commit_message>
download pocketlist by location
</commit_message>
<xml_diff>
--- a/src/main/resources/static/examples/area.xlsx
+++ b/src/main/resources/static/examples/area.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igogo\Documents\資網中心\試場安排\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igogo\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -458,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D436"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A188" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2884,7 +2884,7 @@
         <v>22</v>
       </c>
       <c r="C220">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>